<commit_message>
Working on adding percentages to spreadsheets
</commit_message>
<xml_diff>
--- a/scripts/Half-Elf.xlsx
+++ b/scripts/Half-Elf.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19080" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19080" tabRatio="500" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="15" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="433">
   <si>
     <t>extremely hairy</t>
   </si>
@@ -1337,13 +1337,23 @@
   </si>
   <si>
     <t>drooping</t>
+  </si>
+  <si>
+    <t>Percent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1448,61 +1458,63 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="22">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1524,6 +1536,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="21" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1801,7 +1814,7 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1817,6 +1830,9 @@
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1829,6 +1845,10 @@
         <f>COUNTIF(C$6:C101, "common")</f>
         <v>20</v>
       </c>
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -1842,6 +1862,10 @@
         <f>COUNTIF(C$6:C101, "rare")</f>
         <v>63</v>
       </c>
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>0.1575</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
@@ -2698,7 +2722,7 @@
         <v>0.1</v>
       </c>
       <c r="C70" s="9" t="str">
-        <f t="shared" ref="C70:C101" si="2">IF(B70&gt;=1, "common", "rare")</f>
+        <f t="shared" ref="C70:C88" si="2">IF(B70&gt;=1, "common", "rare")</f>
         <v>rare</v>
       </c>
       <c r="D70" s="10"/>
@@ -2947,10 +2971,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2959,15 +2983,18 @@
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -2978,8 +3005,12 @@
         <f>COUNTIF(C$6:C99, "common")</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -2991,12 +3022,16 @@
         <f>COUNTIF(C$6:C99, "rare")</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>0.30555555555555558</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -3007,7 +3042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -3019,7 +3054,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
@@ -3031,7 +3066,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -3043,7 +3078,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -3055,7 +3090,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
@@ -3067,7 +3102,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -3079,7 +3114,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -3091,7 +3126,7 @@
         <v>rare</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>35</v>
       </c>
@@ -3103,7 +3138,7 @@
         <v>rare</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -3115,7 +3150,7 @@
         <v>rare</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -3127,7 +3162,7 @@
         <v>rare</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -3221,10 +3256,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3233,15 +3268,18 @@
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -3252,8 +3290,12 @@
         <f>COUNTIF(C$6:C99, "common")</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -3265,12 +3307,16 @@
         <f>COUNTIF(C$6:C99, "rare")</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -3281,7 +3327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>407</v>
       </c>
@@ -3293,7 +3339,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>408</v>
       </c>
@@ -3305,7 +3351,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>409</v>
       </c>
@@ -3317,7 +3363,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>410</v>
       </c>
@@ -3329,7 +3375,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>417</v>
       </c>
@@ -3341,7 +3387,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>418</v>
       </c>
@@ -3353,7 +3399,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>424</v>
       </c>
@@ -3365,7 +3411,7 @@
         <v>rare</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>423</v>
       </c>
@@ -3377,7 +3423,7 @@
         <v>rare</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>422</v>
       </c>
@@ -3389,7 +3435,7 @@
         <v>rare</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>421</v>
       </c>
@@ -3401,7 +3447,7 @@
         <v>rare</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>420</v>
       </c>
@@ -3510,7 +3556,7 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3526,6 +3572,9 @@
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -3538,6 +3587,10 @@
         <f>COUNTIF(C$6:C99, "common")</f>
         <v>10</v>
       </c>
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -3550,6 +3603,10 @@
       <c r="C3" s="5">
         <f>COUNTIF(C$6:C99, "rare")</f>
         <v>32</v>
+      </c>
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>0.32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4181,7 +4238,7 @@
   <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4197,6 +4254,9 @@
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -4209,6 +4269,10 @@
         <f>COUNTIF(C$6:C98, "common")</f>
         <v>10</v>
       </c>
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -4221,6 +4285,10 @@
       <c r="C3" s="5">
         <f>COUNTIF(C$6:C98, "rare")</f>
         <v>46</v>
+      </c>
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>0.46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4976,10 +5044,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4988,15 +5056,18 @@
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -5007,8 +5078,12 @@
         <f>COUNTIF(C$6:C98, "common")</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -5020,8 +5095,12 @@
         <f>COUNTIF(C$6:C98, "rare")</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -5032,7 +5111,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
@@ -5044,7 +5123,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>405</v>
       </c>
@@ -5056,7 +5135,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>402</v>
       </c>
@@ -5068,7 +5147,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>404</v>
       </c>
@@ -5080,7 +5159,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>403</v>
       </c>
@@ -5092,7 +5171,7 @@
         <v>rare</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>401</v>
       </c>
@@ -5104,7 +5183,7 @@
         <v>rare</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>2</v>
       </c>
@@ -5116,7 +5195,7 @@
         <v>rare</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>1</v>
       </c>
@@ -5128,7 +5207,7 @@
         <v>rare</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>0</v>
       </c>
@@ -5140,7 +5219,7 @@
         <v>rare</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -5152,7 +5231,7 @@
         <v>rare</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
@@ -5196,8 +5275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5206,15 +5285,18 @@
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -5225,8 +5307,12 @@
         <f>COUNTIF(C$6:C100, "common")</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -5238,11 +5324,15 @@
         <f>COUNTIF(C$6:C100, "rare")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -5253,7 +5343,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -5265,7 +5355,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>406</v>
       </c>
@@ -5277,7 +5367,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -5289,7 +5379,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -5301,7 +5391,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -5313,7 +5403,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -5325,7 +5415,7 @@
         <v>common</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -5337,15 +5427,15 @@
         <v>common</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
     </row>
@@ -5386,7 +5476,7 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5402,6 +5492,9 @@
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -5414,6 +5507,10 @@
         <f>COUNTIF(C$6:C101, "common")</f>
         <v>8</v>
       </c>
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -5426,6 +5523,10 @@
       <c r="C3" s="5">
         <f>COUNTIF(C$6:C101, "rare")</f>
         <v>27</v>
+      </c>
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>0.421875</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -6146,7 +6247,7 @@
   <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6162,6 +6263,9 @@
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -6174,6 +6278,10 @@
         <f>COUNTIF(C$6:C111, "common")</f>
         <v>20</v>
       </c>
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -6186,6 +6294,10 @@
       <c r="C3" s="5">
         <f>COUNTIF(C$7:C111, "rare")</f>
         <v>65</v>
+      </c>
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>0.16250000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -7315,7 +7427,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7331,6 +7443,9 @@
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -7343,6 +7458,10 @@
         <f>COUNTIF(C$6:C99, "common")</f>
         <v>6</v>
       </c>
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -7355,6 +7474,10 @@
       <c r="C3" s="5">
         <f>COUNTIF(C$6:C99, "rare")</f>
         <v>5</v>
+      </c>
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>0.1388888888888889</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -7713,7 +7836,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7729,6 +7852,9 @@
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -7741,6 +7867,10 @@
         <f>COUNTIF(C$6:C99, "common")</f>
         <v>10</v>
       </c>
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -7753,6 +7883,10 @@
       <c r="C3" s="5">
         <f>COUNTIF(C$6:C99, "rare")</f>
         <v>19</v>
+      </c>
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>0.19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -8260,7 +8394,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8276,6 +8410,9 @@
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -8288,6 +8425,10 @@
         <f>COUNTIF(C$6:C99, "common")</f>
         <v>10</v>
       </c>
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -8300,6 +8441,10 @@
       <c r="C3" s="5">
         <f>COUNTIF(C$6:C99, "rare")</f>
         <v>32</v>
+      </c>
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>0.32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -8876,7 +9021,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8892,6 +9037,9 @@
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -8904,6 +9052,10 @@
         <f>COUNTIF(C$6:C98, "common")</f>
         <v>6</v>
       </c>
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -8916,6 +9068,10 @@
       <c r="C3" s="5">
         <f>COUNTIF(C$6:C98, "rare")</f>
         <v>2</v>
+      </c>
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -9178,8 +9334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9195,6 +9351,9 @@
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -9207,6 +9366,10 @@
         <f>COUNTIF(C$6:C99, "common")</f>
         <v>8</v>
       </c>
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -9220,6 +9383,10 @@
         <f>COUNTIF(C$6:C99, "rare")</f>
         <v>23</v>
       </c>
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>0.359375</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
@@ -9244,7 +9411,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="9" t="str">
-        <f>IF(B6&gt;=1, "common", "rare")</f>
+        <f t="shared" ref="C6:C36" si="0">IF(B6&gt;=1, "common", "rare")</f>
         <v>common</v>
       </c>
       <c r="D6" s="7"/>
@@ -9257,7 +9424,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="9" t="str">
-        <f>IF(B7&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>common</v>
       </c>
       <c r="D7" s="7"/>
@@ -9270,7 +9437,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="9" t="str">
-        <f>IF(B8&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>common</v>
       </c>
       <c r="D8" s="7"/>
@@ -9283,7 +9450,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="9" t="str">
-        <f>IF(B9&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>common</v>
       </c>
       <c r="D9" s="7"/>
@@ -9296,7 +9463,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="9" t="str">
-        <f>IF(B10&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>common</v>
       </c>
       <c r="D10" s="7"/>
@@ -9309,7 +9476,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="9" t="str">
-        <f>IF(B11&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>common</v>
       </c>
       <c r="D11" s="7"/>
@@ -9322,7 +9489,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="9" t="str">
-        <f>IF(B12&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>common</v>
       </c>
       <c r="D12" s="7"/>
@@ -9335,7 +9502,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="9" t="str">
-        <f>IF(B13&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>common</v>
       </c>
       <c r="D13" s="7"/>
@@ -9348,7 +9515,7 @@
         <v>0.1</v>
       </c>
       <c r="C14" s="9" t="str">
-        <f>IF(B14&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D14" s="7"/>
@@ -9361,7 +9528,7 @@
         <v>0.1</v>
       </c>
       <c r="C15" s="9" t="str">
-        <f>IF(B15&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D15" s="7"/>
@@ -9374,7 +9541,7 @@
         <v>0.1</v>
       </c>
       <c r="C16" s="9" t="str">
-        <f>IF(B16&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D16" s="7"/>
@@ -9387,7 +9554,7 @@
         <v>0.1</v>
       </c>
       <c r="C17" s="9" t="str">
-        <f>IF(B17&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D17" s="7"/>
@@ -9400,7 +9567,7 @@
         <v>0.1</v>
       </c>
       <c r="C18" s="9" t="str">
-        <f>IF(B18&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D18" s="7"/>
@@ -9413,7 +9580,7 @@
         <v>0.1</v>
       </c>
       <c r="C19" s="9" t="str">
-        <f>IF(B19&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D19" s="2"/>
@@ -9426,7 +9593,7 @@
         <v>0.1</v>
       </c>
       <c r="C20" s="9" t="str">
-        <f>IF(B20&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D20" s="7"/>
@@ -9439,7 +9606,7 @@
         <v>0.1</v>
       </c>
       <c r="C21" s="9" t="str">
-        <f>IF(B21&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D21" s="7"/>
@@ -9452,7 +9619,7 @@
         <v>0.1</v>
       </c>
       <c r="C22" s="9" t="str">
-        <f>IF(B22&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D22" s="7"/>
@@ -9465,7 +9632,7 @@
         <v>0.1</v>
       </c>
       <c r="C23" s="9" t="str">
-        <f>IF(B23&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D23" s="7"/>
@@ -9478,7 +9645,7 @@
         <v>0.1</v>
       </c>
       <c r="C24" s="9" t="str">
-        <f>IF(B24&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D24" s="7"/>
@@ -9491,7 +9658,7 @@
         <v>0.1</v>
       </c>
       <c r="C25" s="9" t="str">
-        <f>IF(B25&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D25" s="7"/>
@@ -9504,7 +9671,7 @@
         <v>0.1</v>
       </c>
       <c r="C26" s="9" t="str">
-        <f>IF(B26&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D26" s="7"/>
@@ -9517,7 +9684,7 @@
         <v>0.1</v>
       </c>
       <c r="C27" s="9" t="str">
-        <f>IF(B27&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D27" s="7"/>
@@ -9530,7 +9697,7 @@
         <v>0.1</v>
       </c>
       <c r="C28" s="9" t="str">
-        <f>IF(B28&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D28" s="7"/>
@@ -9543,7 +9710,7 @@
         <v>0.1</v>
       </c>
       <c r="C29" s="9" t="str">
-        <f>IF(B29&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D29" s="7"/>
@@ -9556,7 +9723,7 @@
         <v>0.1</v>
       </c>
       <c r="C30" s="9" t="str">
-        <f>IF(B30&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D30" s="7"/>
@@ -9569,7 +9736,7 @@
         <v>0.1</v>
       </c>
       <c r="C31" s="9" t="str">
-        <f>IF(B31&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D31" s="7"/>
@@ -9582,7 +9749,7 @@
         <v>0.1</v>
       </c>
       <c r="C32" s="9" t="str">
-        <f>IF(B32&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D32" s="7"/>
@@ -9595,7 +9762,7 @@
         <v>0.1</v>
       </c>
       <c r="C33" s="9" t="str">
-        <f>IF(B33&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D33" s="2"/>
@@ -9608,7 +9775,7 @@
         <v>0.1</v>
       </c>
       <c r="C34" s="9" t="str">
-        <f>IF(B34&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D34" s="2"/>
@@ -9621,7 +9788,7 @@
         <v>0.1</v>
       </c>
       <c r="C35" s="9" t="str">
-        <f>IF(B35&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D35" s="2"/>
@@ -9634,7 +9801,7 @@
         <v>0.1</v>
       </c>
       <c r="C36" s="9" t="str">
-        <f>IF(B36&gt;=1, "common", "rare")</f>
+        <f t="shared" si="0"/>
         <v>rare</v>
       </c>
       <c r="D36" s="2"/>
@@ -9652,7 +9819,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9668,6 +9835,9 @@
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -9680,6 +9850,10 @@
         <f>COUNTIF(C$6:C99, "common")</f>
         <v>8</v>
       </c>
+      <c r="D2" s="15">
+        <f>C2/B2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -9692,6 +9866,10 @@
       <c r="C3" s="5">
         <f>COUNTIF(C$6:C99, "rare")</f>
         <v>11</v>
+      </c>
+      <c r="D3" s="15">
+        <f>C3/B3</f>
+        <v>0.171875</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>